<commit_message>
Max power arc boundary bug Fix
Max power arc boundary calculation pointed to the wrong cell. This version fixed the bug.
</commit_message>
<xml_diff>
--- a/BatteryHazardCalculator_v2.xlsx
+++ b/BatteryHazardCalculator_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmrose\Documents\DCArcFlash\ArcModelValidation\ArcFlashCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1AB581-8546-4E9E-9D34-374A747C16C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398DD49-9B55-4B81-BD6C-1C96EF1623DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4320" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{D4F21237-859F-409A-8BDE-62C477E4C1D5}"/>
+    <workbookView xWindow="-16320" yWindow="-4320" windowWidth="16440" windowHeight="28320" xr2:uid="{D4F21237-859F-409A-8BDE-62C477E4C1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Max Power" sheetId="1" r:id="rId1"/>
@@ -10159,8 +10159,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A7:Y63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10200,7 +10200,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="29">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -10212,7 +10212,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="29">
-        <v>10000</v>
+        <v>2400</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="B13" s="13">
         <f>B11/B12</f>
-        <v>0.05</v>
+        <v>0.21</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>16</v>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="B20" s="8">
         <f>B16*0.01*B11*(B12/2)*B14/((B15)^2)</f>
-        <v>23.919800926021605</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="B21" s="8">
         <f>Y63</f>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
@@ -10325,7 +10325,7 @@
       </c>
       <c r="B22" s="16">
         <f>(B11^2)/(2*B13)</f>
-        <v>2500000</v>
+        <v>604800</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -10387,7 +10387,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="14">
-        <v>6.6660000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>16</v>
@@ -10398,7 +10398,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="10">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
@@ -10420,7 +10420,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>19</v>
@@ -10431,7 +10431,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>19</v>
@@ -10443,7 +10443,7 @@
       </c>
       <c r="B34" s="34">
         <f>(B29*B30+B31*B32)/B33</f>
-        <v>0.13572000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>16</v>
@@ -10455,7 +10455,7 @@
       </c>
       <c r="B35" s="15">
         <f>B11/B34</f>
-        <v>3684.0554081933392</v>
+        <v>2400</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>8</v>
@@ -10497,12 +10497,12 @@
         <v>1</v>
       </c>
       <c r="X38" s="6">
-        <f>B30</f>
-        <v>20</v>
+        <f>B20</f>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y38" s="26">
         <f>$B$15*SQRT(X38/1.2)</f>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -10519,11 +10519,11 @@
       </c>
       <c r="X39" s="26">
         <f>X38/W38*W39</f>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y39" s="26">
         <f>$B$15*SQRT(X39/1.2)</f>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -10539,11 +10539,11 @@
       </c>
       <c r="X40" s="26">
         <f t="shared" ref="X40:X63" si="1">X39/W39*W40</f>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y40" s="26">
         <f t="shared" ref="Y40:Y63" si="2">$B$15*SQRT(X40/1.2)</f>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
@@ -10554,11 +10554,11 @@
       </c>
       <c r="X41" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y41" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
@@ -10568,11 +10568,11 @@
       </c>
       <c r="X42" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y42" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -10582,11 +10582,11 @@
       </c>
       <c r="X43" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y43" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
@@ -10596,11 +10596,11 @@
       </c>
       <c r="X44" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y44" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
@@ -10610,11 +10610,11 @@
       </c>
       <c r="X45" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y45" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
@@ -10624,11 +10624,11 @@
       </c>
       <c r="X46" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y46" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="X47" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y47" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
@@ -10652,11 +10652,11 @@
       </c>
       <c r="X48" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y48" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="49" spans="23:25" x14ac:dyDescent="0.25">
@@ -10666,11 +10666,11 @@
       </c>
       <c r="X49" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y49" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="50" spans="23:25" x14ac:dyDescent="0.25">
@@ -10680,11 +10680,11 @@
       </c>
       <c r="X50" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y50" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="51" spans="23:25" x14ac:dyDescent="0.25">
@@ -10694,11 +10694,11 @@
       </c>
       <c r="X51" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y51" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="52" spans="23:25" x14ac:dyDescent="0.25">
@@ -10708,11 +10708,11 @@
       </c>
       <c r="X52" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y52" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="53" spans="23:25" x14ac:dyDescent="0.25">
@@ -10722,11 +10722,11 @@
       </c>
       <c r="X53" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y53" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="54" spans="23:25" x14ac:dyDescent="0.25">
@@ -10736,11 +10736,11 @@
       </c>
       <c r="X54" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y54" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="55" spans="23:25" x14ac:dyDescent="0.25">
@@ -10750,11 +10750,11 @@
       </c>
       <c r="X55" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y55" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="56" spans="23:25" x14ac:dyDescent="0.25">
@@ -10764,11 +10764,11 @@
       </c>
       <c r="X56" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y56" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="57" spans="23:25" x14ac:dyDescent="0.25">
@@ -10778,11 +10778,11 @@
       </c>
       <c r="X57" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y57" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="58" spans="23:25" x14ac:dyDescent="0.25">
@@ -10792,11 +10792,11 @@
       </c>
       <c r="X58" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y58" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="59" spans="23:25" x14ac:dyDescent="0.25">
@@ -10806,11 +10806,11 @@
       </c>
       <c r="X59" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y59" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="60" spans="23:25" x14ac:dyDescent="0.25">
@@ -10820,11 +10820,11 @@
       </c>
       <c r="X60" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y60" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="61" spans="23:25" x14ac:dyDescent="0.25">
@@ -10834,11 +10834,11 @@
       </c>
       <c r="X61" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y61" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="62" spans="23:25" x14ac:dyDescent="0.25">
@@ -10848,11 +10848,11 @@
       </c>
       <c r="X62" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y62" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
     <row r="63" spans="23:25" x14ac:dyDescent="0.25">
@@ -10862,11 +10862,11 @@
       </c>
       <c r="X63" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.7866782400231465</v>
       </c>
       <c r="Y63" s="26">
         <f t="shared" si="2"/>
-        <v>186.65111840007819</v>
+        <v>100.39920318408907</v>
       </c>
     </row>
   </sheetData>
@@ -10998,7 +10998,7 @@
   <dimension ref="A2:AC63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12693,8 +12693,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A7:BD134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BC74" sqref="BC74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15091,7 +15091,7 @@
         <v>293.47072754061014</v>
       </c>
       <c r="AD74" s="26">
-        <f t="shared" ref="AD73:AD98" si="16">IF(B$20="Inline",0.5*B$23*($AC74-$B$16)/EXP(B$23*($AC74-$B$37)),0.5*B$23/EXP(B$23*B$40))</f>
+        <f t="shared" ref="AD74:AD97" si="16">IF(B$20="Inline",0.5*B$23*($AC74-$B$16)/EXP(B$23*($AC74-$B$37)),0.5*B$23/EXP(B$23*B$40))</f>
         <v>2.7975907561814335</v>
       </c>
       <c r="AE74" s="26">

</xml_diff>